<commit_message>
Assertion added for HealtRisk Assessment
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/inputdata.xlsx
+++ b/qa/src/main/resources/inputdata.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UserData" sheetId="1" r:id="rId1"/>
+    <sheet name="HealtAssessmentData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PatientEmailid</t>
   </si>
@@ -28,7 +29,16 @@
     <t>UserName</t>
   </si>
   <si>
+    <t>Completed_Status</t>
+  </si>
+  <si>
+    <t>InCompleted_Status</t>
+  </si>
+  <si>
     <t>Anas</t>
+  </si>
+  <si>
+    <t>completed on 04.01.2016</t>
   </si>
 </sst>
 </file>
@@ -383,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +423,7 @@
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -423,4 +433,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change maven project to Gradle project
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/inputdata.xlsx
+++ b/qa/src/main/resources/inputdata.xlsx
@@ -38,7 +38,7 @@
     <t>Anas</t>
   </si>
   <si>
-    <t>completed on 03.31.2016</t>
+    <t>completed on 04.01.2016</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>